<commit_message>
Ajustes en modelo y diccionario de datos.
</commit_message>
<xml_diff>
--- a/Documentacion/Tablas/RequerimientosVScasosUso.xlsx
+++ b/Documentacion/Tablas/RequerimientosVScasosUso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28340" yWindow="1420" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -376,8 +376,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -475,7 +483,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -494,6 +502,10 @@
     <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -512,6 +524,10 @@
     <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -844,7 +860,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -983,7 +999,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="17"/>
@@ -1000,7 +1016,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="17"/>
@@ -1017,7 +1033,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="17"/>
@@ -1034,7 +1050,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
       <c r="A10" s="17"/>

</xml_diff>